<commit_message>
úprava samolepek na PCB
</commit_message>
<xml_diff>
--- a/DOC/src/Samolepka_PCB.xlsx
+++ b/DOC/src/Samolepka_PCB.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UST_G\MRAKOMER4\DOC\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UST_G\MRAKOMER04\DOC\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB193228-B5B4-4547-B18C-805FA1E531C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1224182-A5EA-41E8-B1F9-0F3EACE8B67A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="4">
   <si>
     <t>SCL-BROWN</t>
   </si>
@@ -455,20 +455,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:D47"/>
+  <dimension ref="B3:L74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="12.6640625" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" customWidth="1"/>
+    <col min="6" max="6" width="11" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" customWidth="1"/>
+    <col min="9" max="9" width="11" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" customWidth="1"/>
+    <col min="12" max="12" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
@@ -476,8 +482,26 @@
         <v>3</v>
       </c>
       <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
@@ -485,242 +509,1133 @@
         <v>0</v>
       </c>
       <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E8" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E11" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E14" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="L14" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="E17" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="L17" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L19" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="E20" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="K20" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="L20" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B22" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L22" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="E23" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="K23" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="L23" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B25" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="26" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E25" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L25" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="E26" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="K26" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="L26" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B28" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="29" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E28" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L28" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B29" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="E29" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="K29" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="L29" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B31" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="32" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E31" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L31" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B32" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="E32" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I32" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="K32" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="L32" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="34" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B34" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="35" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E34" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L34" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B35" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="E35" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I35" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="K35" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="L35" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="37" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B37" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="38" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E37" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I37" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L37" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B38" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="E38" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I38" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="K38" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="L38" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="40" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B40" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="41" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E40" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I40" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K40" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L40" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B41" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="E41" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H41" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I41" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="K41" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="L41" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="43" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B43" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="44" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E43" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I43" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K43" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L43" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B44" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="E44" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H44" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I44" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="K44" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="L44" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="46" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B46" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="47" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E46" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I46" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K46" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L46" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B47" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C47" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H47" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I47" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="K47" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="L47" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="49" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E49" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I49" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K49" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L49" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="5:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E50" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H50" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I50" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="K50" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="L50" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="5:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="52" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E52" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I52" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K52" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L52" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="5:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E53" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H53" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I53" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="K53" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="L53" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="5:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="55" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E55" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H55" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I55" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K55" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L55" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="5:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E56" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H56" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I56" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="K56" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="L56" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="5:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="58" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E58" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F58" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I58" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K58" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L58" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="5:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E59" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F59" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H59" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I59" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="K59" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="L59" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="5:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="61" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E61" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F61" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I61" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K61" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L61" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="5:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E62" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F62" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H62" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I62" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="K62" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="L62" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="5:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="64" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E64" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H64" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I64" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K64" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L64" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="5:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E65" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H65" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I65" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="K65" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="L65" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="5:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="67" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E67" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F67" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H67" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I67" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K67" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L67" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="5:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E68" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H68" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I68" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="K68" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="L68" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="5:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="70" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E70" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F70" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H70" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I70" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K70" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L70" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="5:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E71" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F71" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H71" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I71" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="K71" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="L71" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="5:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="73" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E73" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F73" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H73" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I73" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K73" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L73" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" spans="5:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E74" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F74" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H74" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I74" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="K74" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="L74" s="5" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>